<commit_message>
Change label to the sum of next three months transactions
</commit_message>
<xml_diff>
--- a/data/output/KPIs_baseline.xlsx
+++ b/data/output/KPIs_baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Vie Professionnelle\CDI Dec 2024 - Data Scientist\Entretiens\Quod_Financial\Quod_THA\data\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA0C224-4504-4A04-878C-0E5F7ED6B040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBC1688-F5CD-4512-A72C-E74AC5C53019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="yearly" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="11">
   <si>
     <t>year</t>
   </si>
@@ -50,6 +50,18 @@
   </si>
   <si>
     <t>LinearRegression_MAE</t>
+  </si>
+  <si>
+    <t>RandomForest_RMSE</t>
+  </si>
+  <si>
+    <t>RandomForest_MAE</t>
+  </si>
+  <si>
+    <t>XGBoost_RMSE</t>
+  </si>
+  <si>
+    <t>XGBoost_MAE</t>
   </si>
   <si>
     <t>month</t>
@@ -430,22 +442,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,39 +474,75 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2018</v>
       </c>
       <c r="B2">
-        <v>71.956779267814383</v>
+        <v>119.6881160032126</v>
       </c>
       <c r="C2">
-        <v>36.007610403396782</v>
+        <v>47.464053496104128</v>
       </c>
       <c r="D2">
-        <v>65.754465116605175</v>
+        <v>121.1001143174017</v>
       </c>
       <c r="E2">
-        <v>32.0759627045503</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>47.472240239665886</v>
+      </c>
+      <c r="F2">
+        <v>115.963711897241</v>
+      </c>
+      <c r="G2">
+        <v>46.522076341341958</v>
+      </c>
+      <c r="H2">
+        <v>131.02770609922541</v>
+      </c>
+      <c r="I2">
+        <v>47.539947509765618</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2019</v>
       </c>
       <c r="B3">
-        <v>60.530085890828317</v>
+        <v>91.681240857849971</v>
       </c>
       <c r="C3">
-        <v>29.762024083849731</v>
+        <v>42.383157409069327</v>
       </c>
       <c r="D3">
-        <v>53.991992791668373</v>
+        <v>96.546136412249552</v>
       </c>
       <c r="E3">
-        <v>25.026321053056261</v>
+        <v>40.568198051076742</v>
+      </c>
+      <c r="F3">
+        <v>99.861586782572147</v>
+      </c>
+      <c r="G3">
+        <v>43.07841844186018</v>
+      </c>
+      <c r="H3">
+        <v>118.876158314546</v>
+      </c>
+      <c r="I3">
+        <v>41.571735382080078</v>
       </c>
     </row>
   </sheetData>
@@ -503,26 +552,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -536,8 +577,20 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>2018</v>
       </c>
@@ -545,163 +598,271 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>98.23105910627153</v>
+        <v>128.01218062765369</v>
       </c>
       <c r="D2">
-        <v>41.514185463588888</v>
+        <v>59.239810617286743</v>
       </c>
       <c r="E2">
-        <v>92.528756164647618</v>
+        <v>121.400400707236</v>
       </c>
       <c r="F2">
-        <v>36.471195435943699</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>53.676536205284137</v>
+      </c>
+      <c r="G2">
+        <v>109.1503076420754</v>
+      </c>
+      <c r="H2">
+        <v>53.91372089053386</v>
+      </c>
+      <c r="I2">
+        <v>125.8135284669836</v>
+      </c>
+      <c r="J2">
+        <v>54.218376159667969</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="1">
         <v>5</v>
       </c>
       <c r="C3">
-        <v>74.87816701085103</v>
+        <v>144.83152315971211</v>
       </c>
       <c r="D3">
-        <v>32.210618524682367</v>
+        <v>58.541047250561647</v>
       </c>
       <c r="E3">
-        <v>64.648614551953912</v>
+        <v>128.19440323675391</v>
       </c>
       <c r="F3">
-        <v>26.16114019103351</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>50.473547024985884</v>
+      </c>
+      <c r="G3">
+        <v>116.151754675338</v>
+      </c>
+      <c r="H3">
+        <v>49.796349877073119</v>
+      </c>
+      <c r="I3">
+        <v>143.4372412851697</v>
+      </c>
+      <c r="J3">
+        <v>48.746318817138672</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="1">
         <v>6</v>
       </c>
       <c r="C4">
-        <v>52.486217532789041</v>
+        <v>105.5688452133104</v>
       </c>
       <c r="D4">
-        <v>32.350933752534132</v>
+        <v>44.833430690606349</v>
       </c>
       <c r="E4">
-        <v>45.486987992333511</v>
+        <v>102.0499042201578</v>
       </c>
       <c r="F4">
-        <v>27.74806991095031</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41.268730950166663</v>
+      </c>
+      <c r="G4">
+        <v>97.494239944351847</v>
+      </c>
+      <c r="H4">
+        <v>39.060158745533663</v>
+      </c>
+      <c r="I4">
+        <v>142.58019262199431</v>
+      </c>
+      <c r="J4">
+        <v>41.127918243408203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="1">
         <v>7</v>
       </c>
       <c r="C5">
-        <v>93.589266636505442</v>
+        <v>120.8098395259609</v>
       </c>
       <c r="D5">
-        <v>43.259144835772901</v>
+        <v>45.336057558990191</v>
       </c>
       <c r="E5">
-        <v>82.172248102521252</v>
+        <v>123.6902078540606</v>
       </c>
       <c r="F5">
-        <v>38.065700762307969</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>44.131777967790832</v>
+      </c>
+      <c r="G5">
+        <v>116.7676875350402</v>
+      </c>
+      <c r="H5">
+        <v>44.318756352530571</v>
+      </c>
+      <c r="I5">
+        <v>127.98701411178401</v>
+      </c>
+      <c r="J5">
+        <v>44.413063049316413</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="1">
         <v>8</v>
       </c>
       <c r="C6">
-        <v>68.5513714721762</v>
+        <v>148.36641337101429</v>
       </c>
       <c r="D6">
-        <v>36.284903872228142</v>
+        <v>49.472631690287237</v>
       </c>
       <c r="E6">
-        <v>64.62879276609047</v>
+        <v>151.3596289346371</v>
       </c>
       <c r="F6">
-        <v>31.165400250472</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>49.678335718080938</v>
+      </c>
+      <c r="G6">
+        <v>144.69728364861879</v>
+      </c>
+      <c r="H6">
+        <v>50.861574478866437</v>
+      </c>
+      <c r="I6">
+        <v>151.58670554133371</v>
+      </c>
+      <c r="J6">
+        <v>51.969280242919922</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="1">
         <v>9</v>
       </c>
       <c r="C7">
-        <v>80.180105903254457</v>
+        <v>139.77026628324541</v>
       </c>
       <c r="D7">
-        <v>43.069614285033758</v>
+        <v>53.888282346114657</v>
       </c>
       <c r="E7">
-        <v>76.678969889430959</v>
+        <v>132.17024168156291</v>
       </c>
       <c r="F7">
-        <v>39.103597743554403</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>52.736346364099937</v>
+      </c>
+      <c r="G7">
+        <v>119.6598246527148</v>
+      </c>
+      <c r="H7">
+        <v>49.970598008091628</v>
+      </c>
+      <c r="I7">
+        <v>123.374964380694</v>
+      </c>
+      <c r="J7">
+        <v>50.138618469238281</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="1">
         <v>10</v>
       </c>
       <c r="C8">
-        <v>62.399690323780831</v>
+        <v>100.74531147367161</v>
       </c>
       <c r="D8">
-        <v>34.557103830991728</v>
+        <v>43.218690523318493</v>
       </c>
       <c r="E8">
-        <v>51.028139167757729</v>
+        <v>100.0012538879139</v>
       </c>
       <c r="F8">
-        <v>30.729200769270989</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>43.516787934716362</v>
+      </c>
+      <c r="G8">
+        <v>124.24080554918071</v>
+      </c>
+      <c r="H8">
+        <v>49.341203762274503</v>
+      </c>
+      <c r="I8">
+        <v>124.3075508064574</v>
+      </c>
+      <c r="J8">
+        <v>48.876564025878913</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="1">
         <v>11</v>
       </c>
       <c r="C9">
-        <v>41.727674761221643</v>
+        <v>87.047430562179613</v>
       </c>
       <c r="D9">
-        <v>28.343922439992021</v>
+        <v>37.394039456165579</v>
       </c>
       <c r="E9">
-        <v>42.896922989428802</v>
+        <v>119.6277215743544</v>
       </c>
       <c r="F9">
-        <v>26.95836737010017</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>43.834473112096198</v>
+      </c>
+      <c r="G9">
+        <v>111.9763204800259</v>
+      </c>
+      <c r="H9">
+        <v>44.919172608102897</v>
+      </c>
+      <c r="I9">
+        <v>124.05263263656479</v>
+      </c>
+      <c r="J9">
+        <v>48.237899780273438</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="1">
         <v>12</v>
       </c>
       <c r="C10">
-        <v>62.198301436927238</v>
+        <v>77.272406546156347</v>
       </c>
       <c r="D10">
-        <v>33.775148334297427</v>
+        <v>34.306570480158157</v>
       </c>
       <c r="E10">
-        <v>61.39506527386208</v>
+        <v>101.0829752405792</v>
       </c>
       <c r="F10">
-        <v>33.732513327958813</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>47.972792324143242</v>
+      </c>
+      <c r="G10">
+        <v>95.807680213568716</v>
+      </c>
+      <c r="H10">
+        <v>36.240636186844888</v>
+      </c>
+      <c r="I10">
+        <v>109.2693775721268</v>
+      </c>
+      <c r="J10">
+        <v>40.021797180175781</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>2019</v>
       </c>
@@ -709,160 +870,268 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>53.304346624306497</v>
+        <v>104.0431769730409</v>
       </c>
       <c r="D11">
-        <v>32.699611513638352</v>
+        <v>59.019698711961119</v>
       </c>
       <c r="E11">
-        <v>53.409679276676833</v>
+        <v>133.8202977630217</v>
       </c>
       <c r="F11">
-        <v>31.332854252361312</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>62.608951816333082</v>
+      </c>
+      <c r="G11">
+        <v>143.35769335277379</v>
+      </c>
+      <c r="H11">
+        <v>54.718035258730978</v>
+      </c>
+      <c r="I11">
+        <v>154.11702255307489</v>
+      </c>
+      <c r="J11">
+        <v>46.837833404541023</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="1">
         <v>2</v>
       </c>
       <c r="C12">
-        <v>70.788516043998001</v>
+        <v>96.704859452357496</v>
       </c>
       <c r="D12">
-        <v>30.7588680437166</v>
+        <v>49.617946524455867</v>
       </c>
       <c r="E12">
-        <v>62.097289186929068</v>
+        <v>92.12001047891512</v>
       </c>
       <c r="F12">
-        <v>24.867718754447971</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>39.795271661691388</v>
+      </c>
+      <c r="G12">
+        <v>80.870196443335814</v>
+      </c>
+      <c r="H12">
+        <v>35.431073087450507</v>
+      </c>
+      <c r="I12">
+        <v>82.305004523001216</v>
+      </c>
+      <c r="J12">
+        <v>34.180690765380859</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="1">
         <v>3</v>
       </c>
       <c r="C13">
-        <v>54.797951051785603</v>
+        <v>91.365210566241061</v>
       </c>
       <c r="D13">
-        <v>30.392893445182271</v>
+        <v>48.305832121750079</v>
       </c>
       <c r="E13">
-        <v>47.779856917050012</v>
+        <v>86.038944269490955</v>
       </c>
       <c r="F13">
-        <v>25.396182677778562</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>43.542854836293159</v>
+      </c>
+      <c r="G13">
+        <v>94.728409161921789</v>
+      </c>
+      <c r="H13">
+        <v>47.897649955407452</v>
+      </c>
+      <c r="I13">
+        <v>94.77920476692131</v>
+      </c>
+      <c r="J13">
+        <v>43.217819213867188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="1">
         <v>4</v>
       </c>
       <c r="C14">
-        <v>80.020263872741054</v>
+        <v>104.7472651505151</v>
       </c>
       <c r="D14">
-        <v>33.335614126552088</v>
+        <v>43.919403237892247</v>
       </c>
       <c r="E14">
-        <v>67.893897070969047</v>
+        <v>99.343769894174201</v>
       </c>
       <c r="F14">
-        <v>27.068812465606339</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42.042093618218608</v>
+      </c>
+      <c r="G14">
+        <v>95.886237783405306</v>
+      </c>
+      <c r="H14">
+        <v>46.579477410415613</v>
+      </c>
+      <c r="I14">
+        <v>103.30587357757059</v>
+      </c>
+      <c r="J14">
+        <v>49.130054473876953</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="1">
         <v>5</v>
       </c>
       <c r="C15">
-        <v>76.172696854858316</v>
+        <v>104.342003525731</v>
       </c>
       <c r="D15">
-        <v>29.9919586269862</v>
+        <v>42.825118556544233</v>
       </c>
       <c r="E15">
-        <v>63.785213062533423</v>
+        <v>96.099635629710519</v>
       </c>
       <c r="F15">
-        <v>24.802569815024231</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>38.226639631978337</v>
+      </c>
+      <c r="G15">
+        <v>102.0297977421183</v>
+      </c>
+      <c r="H15">
+        <v>48.639839366739153</v>
+      </c>
+      <c r="I15">
+        <v>107.8918005457319</v>
+      </c>
+      <c r="J15">
+        <v>48.654705047607422</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="1">
         <v>6</v>
       </c>
       <c r="C16">
-        <v>40.850752229741147</v>
+        <v>84.254172603765653</v>
       </c>
       <c r="D16">
-        <v>26.677582147328859</v>
+        <v>36.289813676152548</v>
       </c>
       <c r="E16">
-        <v>35.276940306487539</v>
+        <v>87.071346411617895</v>
       </c>
       <c r="F16">
-        <v>21.139785659508849</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>35.93017885923534</v>
+      </c>
+      <c r="G16">
+        <v>79.080209055120562</v>
+      </c>
+      <c r="H16">
+        <v>38.963987917466497</v>
+      </c>
+      <c r="I16">
+        <v>71.380506847545576</v>
+      </c>
+      <c r="J16">
+        <v>35.552913665771477</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="1">
         <v>7</v>
       </c>
       <c r="C17">
-        <v>43.695282213001697</v>
+        <v>75.872637340651053</v>
       </c>
       <c r="D17">
-        <v>26.43105282336068</v>
+        <v>32.207488555171523</v>
       </c>
       <c r="E17">
-        <v>40.095127234125279</v>
+        <v>85.457088228571735</v>
       </c>
       <c r="F17">
-        <v>21.759329390339438</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>33.562379312579843</v>
+      </c>
+      <c r="G17">
+        <v>90.956539468638709</v>
+      </c>
+      <c r="H17">
+        <v>38.630125550587167</v>
+      </c>
+      <c r="I17">
+        <v>100.2308663162202</v>
+      </c>
+      <c r="J17">
+        <v>37.175048828125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="1">
         <v>8</v>
       </c>
       <c r="C18">
-        <v>60.573432882693673</v>
+        <v>73.045384699989242</v>
       </c>
       <c r="D18">
-        <v>29.478872880314501</v>
+        <v>31.487901691365469</v>
       </c>
       <c r="E18">
-        <v>59.877662563843593</v>
+        <v>86.702328683285401</v>
       </c>
       <c r="F18">
-        <v>25.36268561069091</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>31.724593952156081</v>
+      </c>
+      <c r="G18">
+        <v>95.198418854177973</v>
+      </c>
+      <c r="H18">
+        <v>34.964416191479621</v>
+      </c>
+      <c r="I18">
+        <v>181.05289929672489</v>
+      </c>
+      <c r="J18">
+        <v>39.336032867431641</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="1">
         <v>9</v>
       </c>
       <c r="C19">
-        <v>47.933036479450152</v>
+        <v>77.028749282919762</v>
       </c>
       <c r="D19">
-        <v>27.03781669578526</v>
+        <v>32.595844375957938</v>
       </c>
       <c r="E19">
-        <v>43.97601638034444</v>
+        <v>85.798829455150184</v>
       </c>
       <c r="F19">
-        <v>22.234064146955589</v>
+        <v>33.339528683259942</v>
+      </c>
+      <c r="G19">
+        <v>97.704844068718984</v>
+      </c>
+      <c r="H19">
+        <v>39.407415241252679</v>
+      </c>
+      <c r="I19">
+        <v>140.32093515847879</v>
+      </c>
+      <c r="J19">
+        <v>38.819690704345703</v>
       </c>
     </row>
   </sheetData>
@@ -876,24 +1145,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -907,125 +1179,225 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>75.799692674159729</v>
+        <v>127.0926735032879</v>
       </c>
       <c r="C2">
-        <v>34.994923387554003</v>
+        <v>54.170850292210567</v>
       </c>
       <c r="D2">
-        <v>68.488495584564106</v>
+        <v>117.6863574411686</v>
       </c>
       <c r="E2">
-        <v>29.772954647498711</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>48.446129955631292</v>
+      </c>
+      <c r="F2">
+        <v>107.8400780109031</v>
+      </c>
+      <c r="G2">
+        <v>47.558245255590151</v>
+      </c>
+      <c r="H2">
+        <v>137.53987347992941</v>
+      </c>
+      <c r="I2">
+        <v>48.004520416259773</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>81.73338149586273</v>
+        <v>136.68523605441641</v>
       </c>
       <c r="C3">
-        <v>40.924968689864777</v>
+        <v>49.511784741181422</v>
       </c>
       <c r="D3">
-        <v>75.033532005331381</v>
+        <v>136.18019659414799</v>
       </c>
       <c r="E3">
-        <v>36.153687070953048</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>48.794488583790347</v>
+      </c>
+      <c r="F3">
+        <v>127.63959174172901</v>
+      </c>
+      <c r="G3">
+        <v>48.347685118712313</v>
+      </c>
+      <c r="H3">
+        <v>134.9079836870302</v>
+      </c>
+      <c r="I3">
+        <v>48.803810119628913</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>56.416366725289897</v>
+        <v>88.972076378361848</v>
       </c>
       <c r="C4">
-        <v>32.286729590310827</v>
+        <v>38.341987243789603</v>
       </c>
       <c r="D4">
-        <v>52.08675147756437</v>
+        <v>107.28626641680449</v>
       </c>
       <c r="E4">
-        <v>30.421543897576971</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45.089240707956428</v>
+      </c>
+      <c r="F4">
+        <v>111.3999477769579</v>
+      </c>
+      <c r="G4">
+        <v>43.554196864428079</v>
+      </c>
+      <c r="H4">
+        <v>119.4792043555593</v>
+      </c>
+      <c r="I4">
+        <v>45.749397277832031</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>59.95216505886912</v>
+        <v>97.608863789251814</v>
       </c>
       <c r="C5">
-        <v>31.300494316922691</v>
+        <v>52.403135341598748</v>
       </c>
       <c r="D5">
-        <v>54.631288394208838</v>
+        <v>106.5495387071112</v>
       </c>
       <c r="E5">
-        <v>27.258508118050869</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>48.816708328369977</v>
+      </c>
+      <c r="F5">
+        <v>110.10773267315891</v>
+      </c>
+      <c r="G5">
+        <v>46.093744059698928</v>
+      </c>
+      <c r="H5">
+        <v>115.3191774828129</v>
+      </c>
+      <c r="I5">
+        <v>41.457550048828118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>68.5149707263583</v>
+        <v>98.37539232546014</v>
       </c>
       <c r="C6">
-        <v>30.047884541423599</v>
+        <v>41.061085362262283</v>
       </c>
       <c r="D6">
-        <v>57.918921208617547</v>
+        <v>94.394023241411574</v>
       </c>
       <c r="E6">
-        <v>24.39286215141302</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>38.773685738404403</v>
+      </c>
+      <c r="F6">
+        <v>92.940371105310604</v>
+      </c>
+      <c r="G6">
+        <v>44.776298408511558</v>
+      </c>
+      <c r="H6">
+        <v>95.768927633131611</v>
+      </c>
+      <c r="I6">
+        <v>44.53375244140625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>50.898269065637507</v>
+        <v>75.304531886982019</v>
       </c>
       <c r="C7">
-        <v>27.59004887583605</v>
+        <v>32.087440541157868</v>
       </c>
       <c r="D7">
-        <v>48.354081757913463</v>
+        <v>85.98081672818617</v>
       </c>
       <c r="E7">
-        <v>23.051999996704161</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32.879141959231838</v>
+      </c>
+      <c r="F7">
+        <v>94.507866628548825</v>
+      </c>
+      <c r="G7">
+        <v>37.646161420638528</v>
+      </c>
+      <c r="H7">
+        <v>143.6437786896808</v>
+      </c>
+      <c r="I7">
+        <v>38.407150268554688</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <f>AVERAGE(B2:B7)</f>
-        <v>65.552474291029554</v>
+        <v>104.00646232296002</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" ref="C8:E8" si="0">AVERAGE(C2:C7)</f>
-        <v>32.857508233651991</v>
+        <f t="shared" ref="C8:I8" si="0">AVERAGE(C2:C7)</f>
+        <v>44.596047253700085</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="0"/>
-        <v>59.418845071366626</v>
+        <v>108.01286652147166</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" si="0"/>
-        <v>28.508592647032795</v>
+        <v>43.799899212230713</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="0"/>
+        <v>107.40593132276807</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="0"/>
+        <v>44.66272185459659</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" si="0"/>
+        <v>124.4431575546907</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" si="0"/>
+        <v>44.492696762084961</v>
       </c>
     </row>
   </sheetData>

</xml_diff>